<commit_message>
Update for the salary and things done this week
</commit_message>
<xml_diff>
--- a/Salary/W3 Salaries and Tasks.xlsx
+++ b/Salary/W3 Salaries and Tasks.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <r>
       <rPr>
@@ -173,19 +173,16 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Ideation</t>
-  </si>
-  <si>
     <t xml:space="preserve">Presentation for class</t>
   </si>
   <si>
-    <t xml:space="preserve">Affinity</t>
+    <t xml:space="preserve">Incorporate feedback for presentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ideation distillation</t>
   </si>
   <si>
     <t xml:space="preserve">Present to stakeholders</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Made Personas</t>
   </si>
 </sst>
 </file>
@@ -443,14 +440,14 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.89"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="90.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -468,7 +465,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="n">
-        <v>43384</v>
+        <v>43391</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -573,7 +570,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
         <v>15</v>
       </c>
@@ -590,9 +587,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="6" t="s">
-        <v>19</v>
-      </c>
+      <c r="A21" s="6"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6"/>

</xml_diff>